<commit_message>
ERD van de database
V1.0
</commit_message>
<xml_diff>
--- a/ERD van de database/ERD.xlsx
+++ b/ERD van de database/ERD.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harun\Desktop\school\leerjaar 2\Project\p2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nieuw\OneDrive\School - Radius\Bioscoop_P5\ERD van de database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7258643-945F-4F46-B52A-A2B3BECD5982}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{1D9891E8-22E8-4DE7-BA6A-FB03FF07BEE1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{C3FD993F-B500-41A6-BF36-67B61E503C33}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5955" xr2:uid="{2953BD99-C6EF-4AA5-A28F-F41779FB6E91}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="45">
   <si>
     <t>Voornaam</t>
   </si>
@@ -51,18 +51,9 @@
     <t>Tussenvoegsel</t>
   </si>
   <si>
-    <t>Tijdstip wanneer de ticket is gekocht</t>
-  </si>
-  <si>
     <t>Film history</t>
   </si>
   <si>
-    <t>BeginTijd van de film</t>
-  </si>
-  <si>
-    <t>EindTijd van de film</t>
-  </si>
-  <si>
     <t>Prijs</t>
   </si>
   <si>
@@ -78,15 +69,9 @@
     <t>Zaal_nummer</t>
   </si>
   <si>
-    <t>Datum hoelaat de film wordt gedraait.</t>
-  </si>
-  <si>
     <t>tbl_bioscoopsysteem</t>
   </si>
   <si>
-    <t>Beschikbaar plaatsen normaal // loveseats per zaal</t>
-  </si>
-  <si>
     <t>Aantal_tickets</t>
   </si>
   <si>
@@ -114,22 +99,67 @@
     <t>◊</t>
   </si>
   <si>
-    <t>tbl_bioscoopsysteem (R1)</t>
-  </si>
-  <si>
-    <t>tbl_b_regels (R2)</t>
-  </si>
-  <si>
-    <t>tbl_b_regels1 (R2)</t>
-  </si>
-  <si>
-    <t>tbl_b_regels2 (R2)</t>
-  </si>
-  <si>
-    <t>tbl_b_regels3 (R2)</t>
-  </si>
-  <si>
     <t>Bestelingnummer</t>
+  </si>
+  <si>
+    <t>Capaciteit</t>
+  </si>
+  <si>
+    <t>rijen</t>
+  </si>
+  <si>
+    <t>Type_zaal</t>
+  </si>
+  <si>
+    <t>ticket_barcode</t>
+  </si>
+  <si>
+    <t>BeginTijd</t>
+  </si>
+  <si>
+    <t>EindTijd</t>
+  </si>
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>Aankoopdatum</t>
+  </si>
+  <si>
+    <t>Beschikbaar_plaatsen</t>
+  </si>
+  <si>
+    <t>Opmerking_zaal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datum </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EindTijd </t>
+  </si>
+  <si>
+    <t>tbl_bestellingen</t>
+  </si>
+  <si>
+    <t>tbl_films</t>
+  </si>
+  <si>
+    <t>tbl_zalen</t>
+  </si>
+  <si>
+    <t>Opmerking_film</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tbl_bioscoopsysteem </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tbl_b_regels1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tbl_b_regels2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tbl_b_regels3 </t>
   </si>
 </sst>
 </file>
@@ -507,117 +537,129 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED11C58-8959-4843-BFDC-F3C78BDF11FA}">
-  <dimension ref="A2:K64"/>
+  <dimension ref="A2:P77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="46.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" customWidth="1"/>
+    <col min="14" max="14" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.85546875" customWidth="1"/>
+    <col min="16" max="16" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
@@ -625,312 +667,540 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>27</v>
+      <c r="A21" t="s">
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>27</v>
+      <c r="A23" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" t="s">
-        <v>16</v>
+      <c r="B27" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>28</v>
+      <c r="A29" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="B29" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="H39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B41" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="H41" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M41" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>0</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M42" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>7</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J43" t="s">
+        <v>29</v>
+      </c>
+      <c r="M43" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>1</v>
+      </c>
+      <c r="H44" t="s">
+        <v>15</v>
+      </c>
+      <c r="J44" t="s">
+        <v>30</v>
+      </c>
+      <c r="M44" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>2</v>
+      </c>
+      <c r="H45" t="s">
+        <v>9</v>
+      </c>
+      <c r="J45" t="s">
+        <v>31</v>
+      </c>
+      <c r="M45" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>4</v>
+      </c>
+      <c r="H46" t="s">
+        <v>5</v>
+      </c>
+      <c r="J46" t="s">
+        <v>17</v>
+      </c>
+      <c r="M46" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>6</v>
+      </c>
+      <c r="H47" t="s">
+        <v>11</v>
+      </c>
+      <c r="M47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>8</v>
+      </c>
+      <c r="H48" t="s">
         <v>28</v>
       </c>
-      <c r="B31" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="1" t="s">
+      <c r="M48" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H49" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B53" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C53" s="1"/>
+      <c r="F53" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L53" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N53" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P53" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="55" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B55" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C55" s="3"/>
+      <c r="F55" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J55" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L55" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N55" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P55" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>0</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J56" t="s">
         <v>29</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="L56" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N56" t="s">
+        <v>34</v>
+      </c>
+      <c r="P56" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>7</v>
+      </c>
+      <c r="F57" t="s">
+        <v>15</v>
+      </c>
+      <c r="J57" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="3" t="s">
+      <c r="N57" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>1</v>
+      </c>
+      <c r="F58" t="s">
+        <v>9</v>
+      </c>
+      <c r="J58" t="s">
+        <v>31</v>
+      </c>
+      <c r="N58" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="59" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>2</v>
+      </c>
+      <c r="F59" t="s">
+        <v>5</v>
+      </c>
+      <c r="J59" t="s">
+        <v>40</v>
+      </c>
+      <c r="N59" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>4</v>
+      </c>
+      <c r="F60" t="s">
+        <v>11</v>
+      </c>
+      <c r="N60" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="61" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>6</v>
+      </c>
+      <c r="F61" t="s">
+        <v>28</v>
+      </c>
+      <c r="N61" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="62" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>8</v>
+      </c>
+      <c r="F62" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="68" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B68" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L68" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N68" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P68" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="70" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B70" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H70" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+      <c r="J70" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L70" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N70" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P70" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
         <v>0</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="C71" s="4"/>
+      <c r="F71" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H71" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J71" t="s">
+        <v>29</v>
+      </c>
+      <c r="L71" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N71" t="s">
+        <v>34</v>
+      </c>
+      <c r="P71" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+    <row r="72" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
         <v>7</v>
       </c>
-      <c r="F38" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+      <c r="F72" t="s">
+        <v>15</v>
+      </c>
+      <c r="J72" t="s">
+        <v>30</v>
+      </c>
+      <c r="N72" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
         <v>1</v>
       </c>
-      <c r="F39" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+      <c r="F73" t="s">
+        <v>9</v>
+      </c>
+      <c r="J73" t="s">
+        <v>31</v>
+      </c>
+      <c r="N73" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="74" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
         <v>2</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F74" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+      <c r="J74" t="s">
+        <v>40</v>
+      </c>
+      <c r="N74" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="75" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
         <v>4</v>
       </c>
-      <c r="F41" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+      <c r="F75" t="s">
+        <v>11</v>
+      </c>
+      <c r="N75" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="76" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F44" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F45" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F46" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F47" t="s">
+      <c r="F76" t="s">
+        <v>28</v>
+      </c>
+      <c r="N76" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="77" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F48" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="F50" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="F51" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="F52" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="F53" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B55" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H55" s="1" t="s">
+      <c r="F77" t="s">
         <v>32</v>
-      </c>
-      <c r="K55" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>3</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H57" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K57" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>0</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H58" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K58" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>7</v>
-      </c>
-      <c r="F59" t="s">
-        <v>20</v>
-      </c>
-      <c r="H59" t="s">
-        <v>10</v>
-      </c>
-      <c r="K59" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>1</v>
-      </c>
-      <c r="F60" t="s">
-        <v>12</v>
-      </c>
-      <c r="H60" t="s">
-        <v>11</v>
-      </c>
-      <c r="K60" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
-        <v>2</v>
-      </c>
-      <c r="F61" t="s">
-        <v>5</v>
-      </c>
-      <c r="H61" t="s">
-        <v>17</v>
-      </c>
-      <c r="K61" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>4</v>
-      </c>
-      <c r="F62" t="s">
-        <v>14</v>
-      </c>
-      <c r="H62" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>6</v>
-      </c>
-      <c r="H63" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>